<commit_message>
promo / printing spots uncleaned excels
</commit_message>
<xml_diff>
--- a/exports_b2b_suppliers/yp_janitorial_queens-ny_filtered.xlsx
+++ b/exports_b2b_suppliers/yp_janitorial_queens-ny_filtered.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyalor/.projects/scripts/yp/exports_b2b_suppliers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C95E9F-654F-1641-A637-34EFA84DFFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="238">
   <si>
     <t>#</t>
   </si>
@@ -725,13 +731,16 @@
   </si>
   <si>
     <t>Not Contacted</t>
+  </si>
+  <si>
+    <t>david@twi-laq.com email a proposal, follow up phone call say you want to speak to david</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,12 +764,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -794,12 +815,16 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -807,13 +832,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -851,7 +884,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -885,6 +918,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -919,9 +953,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1094,14 +1129,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="103.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="76.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="91.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,8 +1202,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1186,8 +1240,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1221,8 +1275,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1256,8 +1310,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1294,8 +1348,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1332,8 +1386,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1370,8 +1424,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1401,12 +1455,15 @@
       <c r="M8" s="2" t="s">
         <v>207</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="O8" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1440,8 +1497,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1475,8 +1532,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1510,8 +1567,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
-      <c r="A12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1545,8 +1602,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
-      <c r="A13">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1580,8 +1637,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1615,8 +1672,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1650,8 +1707,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1688,8 +1745,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1723,8 +1780,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1761,8 +1818,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
-      <c r="A19">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1799,8 +1856,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
-      <c r="A20">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1837,8 +1894,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
-      <c r="A21">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1872,8 +1929,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
-      <c r="A22">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1907,8 +1964,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
-      <c r="A23">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1942,8 +1999,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
-      <c r="A24">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1980,8 +2037,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -2015,8 +2072,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -2053,8 +2110,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -2088,8 +2145,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -2126,8 +2183,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -2164,8 +2221,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -2199,8 +2256,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -2237,8 +2294,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
-      <c r="A32">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -2275,8 +2332,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
-      <c r="A33">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -2313,8 +2370,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
-      <c r="A34">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -2351,8 +2408,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
-      <c r="A35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -2389,8 +2446,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
-      <c r="A36">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -2429,76 +2486,77 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
-    <hyperlink ref="I4" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6"/>
-    <hyperlink ref="I5" r:id="rId7"/>
-    <hyperlink ref="M5" r:id="rId8"/>
-    <hyperlink ref="I6" r:id="rId9"/>
-    <hyperlink ref="M6" r:id="rId10"/>
-    <hyperlink ref="I7" r:id="rId11"/>
-    <hyperlink ref="M7" r:id="rId12"/>
-    <hyperlink ref="I8" r:id="rId13"/>
-    <hyperlink ref="M8" r:id="rId14"/>
-    <hyperlink ref="I9" r:id="rId15"/>
-    <hyperlink ref="M9" r:id="rId16"/>
-    <hyperlink ref="I10" r:id="rId17"/>
-    <hyperlink ref="M10" r:id="rId18"/>
-    <hyperlink ref="I11" r:id="rId19"/>
-    <hyperlink ref="M11" r:id="rId20"/>
-    <hyperlink ref="I12" r:id="rId21"/>
-    <hyperlink ref="M12" r:id="rId22"/>
-    <hyperlink ref="I13" r:id="rId23"/>
-    <hyperlink ref="M13" r:id="rId24"/>
-    <hyperlink ref="I14" r:id="rId25"/>
-    <hyperlink ref="M14" r:id="rId26"/>
-    <hyperlink ref="I15" r:id="rId27"/>
-    <hyperlink ref="M15" r:id="rId28"/>
-    <hyperlink ref="I16" r:id="rId29"/>
-    <hyperlink ref="M16" r:id="rId30"/>
-    <hyperlink ref="I17" r:id="rId31"/>
-    <hyperlink ref="M17" r:id="rId32"/>
-    <hyperlink ref="I18" r:id="rId33"/>
-    <hyperlink ref="M18" r:id="rId34"/>
-    <hyperlink ref="I19" r:id="rId35"/>
-    <hyperlink ref="M19" r:id="rId36"/>
-    <hyperlink ref="I20" r:id="rId37"/>
-    <hyperlink ref="M20" r:id="rId38"/>
-    <hyperlink ref="I21" r:id="rId39"/>
-    <hyperlink ref="M21" r:id="rId40"/>
-    <hyperlink ref="I22" r:id="rId41"/>
-    <hyperlink ref="M22" r:id="rId42"/>
-    <hyperlink ref="I23" r:id="rId43"/>
-    <hyperlink ref="M23" r:id="rId44"/>
-    <hyperlink ref="I24" r:id="rId45"/>
-    <hyperlink ref="M24" r:id="rId46"/>
-    <hyperlink ref="I25" r:id="rId47"/>
-    <hyperlink ref="M25" r:id="rId48"/>
-    <hyperlink ref="I26" r:id="rId49"/>
-    <hyperlink ref="M26" r:id="rId50"/>
-    <hyperlink ref="I27" r:id="rId51"/>
-    <hyperlink ref="M27" r:id="rId52"/>
-    <hyperlink ref="I28" r:id="rId53"/>
-    <hyperlink ref="M28" r:id="rId54"/>
-    <hyperlink ref="I29" r:id="rId55"/>
-    <hyperlink ref="M29" r:id="rId56"/>
-    <hyperlink ref="I30" r:id="rId57"/>
-    <hyperlink ref="M30" r:id="rId58"/>
-    <hyperlink ref="I31" r:id="rId59"/>
-    <hyperlink ref="M31" r:id="rId60"/>
-    <hyperlink ref="I32" r:id="rId61"/>
-    <hyperlink ref="M32" r:id="rId62"/>
-    <hyperlink ref="I33" r:id="rId63"/>
-    <hyperlink ref="M33" r:id="rId64"/>
-    <hyperlink ref="I34" r:id="rId65"/>
-    <hyperlink ref="M34" r:id="rId66"/>
-    <hyperlink ref="I35" r:id="rId67"/>
-    <hyperlink ref="M35" r:id="rId68"/>
-    <hyperlink ref="I36" r:id="rId69"/>
-    <hyperlink ref="M36" r:id="rId70"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="M5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="M6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="M7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="M8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="M9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="M10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="M11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="M12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="I13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="M14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="I15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="M15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="I16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="M16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="M17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="M18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="I19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="M19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="I20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="M20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="I21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="I22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="M22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="I23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="M23" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="I24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="M24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="I25" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="M25" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="I26" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="M26" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="I27" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="M27" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="I28" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="M28" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="I29" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="M29" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="I30" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="M30" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="I31" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="M31" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="I32" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="M32" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="I33" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="M33" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="I34" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="M34" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="I35" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="M35" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="I36" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="M36" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="N8" r:id="rId71" xr:uid="{C87F2188-0166-8849-8FAD-C0F81C54F817}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>